<commit_message>
Updated header files so that the app shows a different header depending on whether you're logged in; added login/register text to main page; updated testing spreadsheet
</commit_message>
<xml_diff>
--- a/project-documents/testing/v2/moodTube Testing Spreadsheet v2.xlsx
+++ b/project-documents/testing/v2/moodTube Testing Spreadsheet v2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sonya\Documents\Sonya's Documents\moodtube\project-documents\testing\v1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sonya\Documents\Sonya's Documents\moodtube\project-documents\testing\v2\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="143">
   <si>
     <t>Form Field Validations</t>
   </si>
@@ -438,6 +438,21 @@
   </si>
   <si>
     <t>need to add an error message if email is not unique for registration</t>
+  </si>
+  <si>
+    <t>system allows user to enter any value for email when that's not correct</t>
+  </si>
+  <si>
+    <t>clicking like dislike share or unlike or undislike reroutes the user instead of letting them continue the search</t>
+  </si>
+  <si>
+    <t>buttons for logged-in only functions show for unlogged in users</t>
+  </si>
+  <si>
+    <t>share button doesn't work</t>
+  </si>
+  <si>
+    <t>Jordan</t>
   </si>
 </sst>
 </file>
@@ -765,10 +780,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H62"/>
+  <dimension ref="A1:H66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C62" sqref="C62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1661,14 +1676,17 @@
       <c r="D60">
         <v>1</v>
       </c>
+      <c r="E60" t="s">
+        <v>124</v>
+      </c>
+      <c r="F60" s="2">
+        <v>43071</v>
+      </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>10</v>
       </c>
-      <c r="B61" t="s">
-        <v>112</v>
-      </c>
       <c r="C61" t="s">
         <v>136</v>
       </c>
@@ -1685,6 +1703,65 @@
       </c>
       <c r="D62">
         <v>3</v>
+      </c>
+      <c r="E62" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <v>12</v>
+      </c>
+      <c r="C63" t="s">
+        <v>138</v>
+      </c>
+      <c r="D63">
+        <v>3</v>
+      </c>
+      <c r="E63" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <v>13</v>
+      </c>
+      <c r="C64" t="s">
+        <v>139</v>
+      </c>
+      <c r="D64">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A65">
+        <v>14</v>
+      </c>
+      <c r="C65" t="s">
+        <v>140</v>
+      </c>
+      <c r="D65">
+        <v>2</v>
+      </c>
+      <c r="E65" t="s">
+        <v>113</v>
+      </c>
+      <c r="F65" s="2">
+        <v>43071</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <v>15</v>
+      </c>
+      <c r="C66" t="s">
+        <v>141</v>
+      </c>
+      <c r="D66">
+        <v>2</v>
+      </c>
+      <c r="E66" t="s">
+        <v>142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated heading references, removed buttons for 'analyze tweets' and 'no twitter?' from page for un-logged in users; more testing.
</commit_message>
<xml_diff>
--- a/project-documents/testing/v2/moodTube Testing Spreadsheet v2.xlsx
+++ b/project-documents/testing/v2/moodTube Testing Spreadsheet v2.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="148">
   <si>
     <t>Form Field Validations</t>
   </si>
@@ -453,6 +453,21 @@
   </si>
   <si>
     <t>Jordan</t>
+  </si>
+  <si>
+    <t>failed login attempt routes to a blank page that only says try again or make an account</t>
+  </si>
+  <si>
+    <t>app wouldn't run because of faulty html syntax</t>
+  </si>
+  <si>
+    <t>Sonya/Ryan</t>
+  </si>
+  <si>
+    <t>wrong header displays on login, register, moodchoose, likes, dislikes pages</t>
+  </si>
+  <si>
+    <t>if you log out, and then attempt to log back in but put the wrong password, internal service error</t>
   </si>
 </sst>
 </file>
@@ -780,10 +795,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H66"/>
+  <dimension ref="A1:H70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C62" sqref="C62"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1744,7 +1759,7 @@
         <v>2</v>
       </c>
       <c r="E65" t="s">
-        <v>113</v>
+        <v>145</v>
       </c>
       <c r="F65" s="2">
         <v>43071</v>
@@ -1762,6 +1777,62 @@
       </c>
       <c r="E66" t="s">
         <v>142</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <v>16</v>
+      </c>
+      <c r="C67" t="s">
+        <v>143</v>
+      </c>
+      <c r="D67">
+        <v>1</v>
+      </c>
+      <c r="E67" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <v>17</v>
+      </c>
+      <c r="C68" t="s">
+        <v>144</v>
+      </c>
+      <c r="D68">
+        <v>1</v>
+      </c>
+      <c r="E68" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <v>18</v>
+      </c>
+      <c r="C69" t="s">
+        <v>146</v>
+      </c>
+      <c r="D69">
+        <v>1</v>
+      </c>
+      <c r="E69" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <v>19</v>
+      </c>
+      <c r="C70" t="s">
+        <v>147</v>
+      </c>
+      <c r="D70">
+        <v>2</v>
+      </c>
+      <c r="E70" t="s">
+        <v>124</v>
       </c>
     </row>
   </sheetData>

</xml_diff>